<commit_message>
changed usa pop 1950
</commit_message>
<xml_diff>
--- a/usa_pop.xlsx
+++ b/usa_pop.xlsx
@@ -116,7 +116,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -145,7 +145,7 @@
         <v>1950</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="4">

</xml_diff>